<commit_message>
Updated Metrics, Backlog and Burndown Chart
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Burndown Chart.xlsx
+++ b/Project/Phase 2/Sprint1/Burndown Chart.xlsx
@@ -5,24 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntiMach\Desktop\uni-workspace\ES\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmtbl\Documents\GitHub\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC60C8FF-667F-415A-BE8F-C5EA6B991047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9C76AE-6701-452A-82E3-80D22CCAE166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>BackLog ID</t>
   </si>
@@ -63,6 +66,9 @@
   </si>
   <si>
     <t>Pedro Lopes</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
   </si>
 </sst>
 </file>
@@ -317,6 +323,10 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -334,10 +344,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,28 +455,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4.3999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4.3999999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,25 +541,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.2857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.8571428571428572</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.1428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.4285714285714284</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.71428571428571441</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -964,7 +970,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1028,19 +1034,29 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4">
+        <v>0.2</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1050,8 +1066,12 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -1061,8 +1081,12 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1072,14 +1096,20 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4">
+        <v>0.4</v>
+      </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1088,35 +1118,35 @@
       </c>
       <c r="B8" s="6">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" ref="C8:I8" si="0">B8-SUM(C3:C7)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.3999999999999995</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.3999999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1125,31 +1155,31 @@
       </c>
       <c r="B9" s="8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C9" s="9">
         <f>B9-(B9/7*C2)</f>
-        <v>0</v>
+        <v>4.2857142857142856</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" ref="D9:I9" si="1">$B9-($B9/7*D2)</f>
-        <v>0</v>
+        <v>3.5714285714285712</v>
       </c>
       <c r="E9" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4285714285714284</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.71428571428571441</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="1"/>
@@ -1201,10 +1231,10 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="21"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -1213,8 +1243,10 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="23"/>
       <c r="D15" s="15" t="s">
         <v>5</v>
       </c>
@@ -1225,8 +1257,10 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="25"/>
       <c r="D16" s="16" t="s">
         <v>6</v>
       </c>
@@ -1237,22 +1271,28 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="25"/>
       <c r="D17" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="25"/>
       <c r="D18" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="25"/>
       <c r="D19" s="19" t="s">
         <v>9</v>
       </c>
@@ -2240,12 +2280,12 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>